<commit_message>
seeded draft results data, created route of draft results
</commit_message>
<xml_diff>
--- a/db/seeds/draft_results_worksheet.xlsx
+++ b/db/seeds/draft_results_worksheet.xlsx
@@ -1755,7 +1755,7 @@
   <dimension ref="A1:J302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1770,10 +1770,10 @@
         <v>469</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
       </c>
       <c r="D1" t="s">
         <v>163</v>
@@ -1822,10 +1822,10 @@
         <v>2015</v>
       </c>
       <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
         <v>1</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -1848,10 +1848,10 @@
         <v>2015</v>
       </c>
       <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
         <v>1</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -1874,10 +1874,10 @@
         <v>2015</v>
       </c>
       <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
         <v>1</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1900,10 +1900,10 @@
         <v>2015</v>
       </c>
       <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
         <v>1</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -1926,10 +1926,10 @@
         <v>2015</v>
       </c>
       <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
         <v>1</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -1952,10 +1952,10 @@
         <v>2015</v>
       </c>
       <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
         <v>1</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -1978,10 +1978,10 @@
         <v>2015</v>
       </c>
       <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
         <v>1</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -2004,10 +2004,10 @@
         <v>2015</v>
       </c>
       <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
         <v>1</v>
-      </c>
-      <c r="C10">
-        <v>9</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -2030,10 +2030,10 @@
         <v>2015</v>
       </c>
       <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
         <v>1</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -2056,10 +2056,10 @@
         <v>2015</v>
       </c>
       <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
         <v>2</v>
-      </c>
-      <c r="C12">
-        <v>11</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -2082,10 +2082,10 @@
         <v>2015</v>
       </c>
       <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
         <v>2</v>
-      </c>
-      <c r="C13">
-        <v>12</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
@@ -2108,10 +2108,10 @@
         <v>2015</v>
       </c>
       <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
         <v>2</v>
-      </c>
-      <c r="C14">
-        <v>13</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
@@ -2134,10 +2134,10 @@
         <v>2015</v>
       </c>
       <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
         <v>2</v>
-      </c>
-      <c r="C15">
-        <v>14</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
@@ -2160,10 +2160,10 @@
         <v>2015</v>
       </c>
       <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
         <v>2</v>
-      </c>
-      <c r="C16">
-        <v>15</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
@@ -2186,10 +2186,10 @@
         <v>2015</v>
       </c>
       <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
         <v>2</v>
-      </c>
-      <c r="C17">
-        <v>16</v>
       </c>
       <c r="D17" t="s">
         <v>3</v>
@@ -2212,10 +2212,10 @@
         <v>2015</v>
       </c>
       <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
         <v>2</v>
-      </c>
-      <c r="C18">
-        <v>17</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
@@ -2238,10 +2238,10 @@
         <v>2015</v>
       </c>
       <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
         <v>2</v>
-      </c>
-      <c r="C19">
-        <v>18</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
@@ -2264,10 +2264,10 @@
         <v>2015</v>
       </c>
       <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
         <v>2</v>
-      </c>
-      <c r="C20">
-        <v>19</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -2290,10 +2290,10 @@
         <v>2015</v>
       </c>
       <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
         <v>2</v>
-      </c>
-      <c r="C21">
-        <v>20</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -2316,10 +2316,10 @@
         <v>2015</v>
       </c>
       <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
         <v>3</v>
-      </c>
-      <c r="C22">
-        <v>21</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -2342,10 +2342,10 @@
         <v>2015</v>
       </c>
       <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
         <v>3</v>
-      </c>
-      <c r="C23">
-        <v>22</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
@@ -2368,10 +2368,10 @@
         <v>2015</v>
       </c>
       <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
         <v>3</v>
-      </c>
-      <c r="C24">
-        <v>23</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
@@ -2394,10 +2394,10 @@
         <v>2015</v>
       </c>
       <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
         <v>3</v>
-      </c>
-      <c r="C25">
-        <v>24</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
@@ -2420,10 +2420,10 @@
         <v>2015</v>
       </c>
       <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
         <v>3</v>
-      </c>
-      <c r="C26">
-        <v>25</v>
       </c>
       <c r="D26" t="s">
         <v>3</v>
@@ -2446,10 +2446,10 @@
         <v>2015</v>
       </c>
       <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
         <v>3</v>
-      </c>
-      <c r="C27">
-        <v>26</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
@@ -2472,10 +2472,10 @@
         <v>2015</v>
       </c>
       <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
         <v>3</v>
-      </c>
-      <c r="C28">
-        <v>27</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
@@ -2498,10 +2498,10 @@
         <v>2015</v>
       </c>
       <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
         <v>3</v>
-      </c>
-      <c r="C29">
-        <v>28</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
@@ -2524,10 +2524,10 @@
         <v>2015</v>
       </c>
       <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
         <v>3</v>
-      </c>
-      <c r="C30">
-        <v>29</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
@@ -2550,10 +2550,10 @@
         <v>2015</v>
       </c>
       <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
         <v>3</v>
-      </c>
-      <c r="C31">
-        <v>30</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -2576,10 +2576,10 @@
         <v>2015</v>
       </c>
       <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
         <v>4</v>
-      </c>
-      <c r="C32">
-        <v>31</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
@@ -2602,10 +2602,10 @@
         <v>2015</v>
       </c>
       <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
         <v>4</v>
-      </c>
-      <c r="C33">
-        <v>32</v>
       </c>
       <c r="D33" t="s">
         <v>4</v>
@@ -2628,10 +2628,10 @@
         <v>2015</v>
       </c>
       <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
         <v>4</v>
-      </c>
-      <c r="C34">
-        <v>33</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
@@ -2654,10 +2654,10 @@
         <v>2015</v>
       </c>
       <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
         <v>4</v>
-      </c>
-      <c r="C35">
-        <v>34</v>
       </c>
       <c r="D35" t="s">
         <v>6</v>
@@ -2680,10 +2680,10 @@
         <v>2015</v>
       </c>
       <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
         <v>4</v>
-      </c>
-      <c r="C36">
-        <v>35</v>
       </c>
       <c r="D36" t="s">
         <v>5</v>
@@ -2706,10 +2706,10 @@
         <v>2015</v>
       </c>
       <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
         <v>4</v>
-      </c>
-      <c r="C37">
-        <v>36</v>
       </c>
       <c r="D37" t="s">
         <v>3</v>
@@ -2732,10 +2732,10 @@
         <v>2015</v>
       </c>
       <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38">
         <v>4</v>
-      </c>
-      <c r="C38">
-        <v>37</v>
       </c>
       <c r="D38" t="s">
         <v>9</v>
@@ -2758,10 +2758,10 @@
         <v>2015</v>
       </c>
       <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39">
         <v>4</v>
-      </c>
-      <c r="C39">
-        <v>38</v>
       </c>
       <c r="D39" t="s">
         <v>8</v>
@@ -2784,10 +2784,10 @@
         <v>2015</v>
       </c>
       <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40">
         <v>4</v>
-      </c>
-      <c r="C40">
-        <v>39</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -2810,10 +2810,10 @@
         <v>2015</v>
       </c>
       <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
         <v>4</v>
-      </c>
-      <c r="C41">
-        <v>40</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -2836,10 +2836,10 @@
         <v>2015</v>
       </c>
       <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42">
         <v>5</v>
-      </c>
-      <c r="C42">
-        <v>41</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
@@ -2862,10 +2862,10 @@
         <v>2015</v>
       </c>
       <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43">
         <v>5</v>
-      </c>
-      <c r="C43">
-        <v>42</v>
       </c>
       <c r="D43" t="s">
         <v>7</v>
@@ -2888,10 +2888,10 @@
         <v>2015</v>
       </c>
       <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44">
         <v>5</v>
-      </c>
-      <c r="C44">
-        <v>43</v>
       </c>
       <c r="D44" t="s">
         <v>8</v>
@@ -2914,10 +2914,10 @@
         <v>2015</v>
       </c>
       <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45">
         <v>5</v>
-      </c>
-      <c r="C45">
-        <v>44</v>
       </c>
       <c r="D45" t="s">
         <v>9</v>
@@ -2940,10 +2940,10 @@
         <v>2015</v>
       </c>
       <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46">
         <v>5</v>
-      </c>
-      <c r="C46">
-        <v>45</v>
       </c>
       <c r="D46" t="s">
         <v>3</v>
@@ -2966,10 +2966,10 @@
         <v>2015</v>
       </c>
       <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47">
         <v>5</v>
-      </c>
-      <c r="C47">
-        <v>46</v>
       </c>
       <c r="D47" t="s">
         <v>5</v>
@@ -2992,10 +2992,10 @@
         <v>2015</v>
       </c>
       <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48">
         <v>5</v>
-      </c>
-      <c r="C48">
-        <v>47</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
@@ -3018,10 +3018,10 @@
         <v>2015</v>
       </c>
       <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49">
         <v>5</v>
-      </c>
-      <c r="C49">
-        <v>48</v>
       </c>
       <c r="D49" t="s">
         <v>10</v>
@@ -3044,10 +3044,10 @@
         <v>2015</v>
       </c>
       <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50">
         <v>5</v>
-      </c>
-      <c r="C50">
-        <v>49</v>
       </c>
       <c r="D50" t="s">
         <v>4</v>
@@ -3070,10 +3070,10 @@
         <v>2015</v>
       </c>
       <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51">
         <v>5</v>
-      </c>
-      <c r="C51">
-        <v>50</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
@@ -3096,10 +3096,10 @@
         <v>2015</v>
       </c>
       <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52">
         <v>6</v>
-      </c>
-      <c r="C52">
-        <v>51</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
@@ -3122,10 +3122,10 @@
         <v>2015</v>
       </c>
       <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53">
         <v>6</v>
-      </c>
-      <c r="C53">
-        <v>52</v>
       </c>
       <c r="D53" t="s">
         <v>4</v>
@@ -3148,10 +3148,10 @@
         <v>2015</v>
       </c>
       <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54">
         <v>6</v>
-      </c>
-      <c r="C54">
-        <v>53</v>
       </c>
       <c r="D54" t="s">
         <v>10</v>
@@ -3174,10 +3174,10 @@
         <v>2015</v>
       </c>
       <c r="B55">
+        <v>54</v>
+      </c>
+      <c r="C55">
         <v>6</v>
-      </c>
-      <c r="C55">
-        <v>54</v>
       </c>
       <c r="D55" t="s">
         <v>6</v>
@@ -3200,10 +3200,10 @@
         <v>2015</v>
       </c>
       <c r="B56">
+        <v>55</v>
+      </c>
+      <c r="C56">
         <v>6</v>
-      </c>
-      <c r="C56">
-        <v>55</v>
       </c>
       <c r="D56" t="s">
         <v>5</v>
@@ -3226,10 +3226,10 @@
         <v>2015</v>
       </c>
       <c r="B57">
+        <v>56</v>
+      </c>
+      <c r="C57">
         <v>6</v>
-      </c>
-      <c r="C57">
-        <v>56</v>
       </c>
       <c r="D57" t="s">
         <v>3</v>
@@ -3252,10 +3252,10 @@
         <v>2015</v>
       </c>
       <c r="B58">
+        <v>57</v>
+      </c>
+      <c r="C58">
         <v>6</v>
-      </c>
-      <c r="C58">
-        <v>57</v>
       </c>
       <c r="D58" t="s">
         <v>9</v>
@@ -3278,10 +3278,10 @@
         <v>2015</v>
       </c>
       <c r="B59">
+        <v>58</v>
+      </c>
+      <c r="C59">
         <v>6</v>
-      </c>
-      <c r="C59">
-        <v>58</v>
       </c>
       <c r="D59" t="s">
         <v>8</v>
@@ -3304,10 +3304,10 @@
         <v>2015</v>
       </c>
       <c r="B60">
+        <v>59</v>
+      </c>
+      <c r="C60">
         <v>6</v>
-      </c>
-      <c r="C60">
-        <v>59</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
@@ -3330,10 +3330,10 @@
         <v>2015</v>
       </c>
       <c r="B61">
+        <v>60</v>
+      </c>
+      <c r="C61">
         <v>6</v>
-      </c>
-      <c r="C61">
-        <v>60</v>
       </c>
       <c r="D61" t="s">
         <v>11</v>
@@ -3356,10 +3356,10 @@
         <v>2015</v>
       </c>
       <c r="B62">
+        <v>61</v>
+      </c>
+      <c r="C62">
         <v>7</v>
-      </c>
-      <c r="C62">
-        <v>61</v>
       </c>
       <c r="D62" t="s">
         <v>11</v>
@@ -3382,10 +3382,10 @@
         <v>2015</v>
       </c>
       <c r="B63">
+        <v>62</v>
+      </c>
+      <c r="C63">
         <v>7</v>
-      </c>
-      <c r="C63">
-        <v>62</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
@@ -3408,10 +3408,10 @@
         <v>2015</v>
       </c>
       <c r="B64">
+        <v>63</v>
+      </c>
+      <c r="C64">
         <v>7</v>
-      </c>
-      <c r="C64">
-        <v>63</v>
       </c>
       <c r="D64" t="s">
         <v>8</v>
@@ -3434,10 +3434,10 @@
         <v>2015</v>
       </c>
       <c r="B65">
+        <v>64</v>
+      </c>
+      <c r="C65">
         <v>7</v>
-      </c>
-      <c r="C65">
-        <v>64</v>
       </c>
       <c r="D65" t="s">
         <v>9</v>
@@ -3460,10 +3460,10 @@
         <v>2015</v>
       </c>
       <c r="B66">
+        <v>65</v>
+      </c>
+      <c r="C66">
         <v>7</v>
-      </c>
-      <c r="C66">
-        <v>65</v>
       </c>
       <c r="D66" t="s">
         <v>3</v>
@@ -3486,10 +3486,10 @@
         <v>2015</v>
       </c>
       <c r="B67">
+        <v>66</v>
+      </c>
+      <c r="C67">
         <v>7</v>
-      </c>
-      <c r="C67">
-        <v>66</v>
       </c>
       <c r="D67" t="s">
         <v>5</v>
@@ -3512,10 +3512,10 @@
         <v>2015</v>
       </c>
       <c r="B68">
+        <v>67</v>
+      </c>
+      <c r="C68">
         <v>7</v>
-      </c>
-      <c r="C68">
-        <v>67</v>
       </c>
       <c r="D68" t="s">
         <v>6</v>
@@ -3538,10 +3538,10 @@
         <v>2015</v>
       </c>
       <c r="B69">
+        <v>68</v>
+      </c>
+      <c r="C69">
         <v>7</v>
-      </c>
-      <c r="C69">
-        <v>68</v>
       </c>
       <c r="D69" t="s">
         <v>10</v>
@@ -3564,10 +3564,10 @@
         <v>2015</v>
       </c>
       <c r="B70">
+        <v>69</v>
+      </c>
+      <c r="C70">
         <v>7</v>
-      </c>
-      <c r="C70">
-        <v>69</v>
       </c>
       <c r="D70" t="s">
         <v>4</v>
@@ -3590,10 +3590,10 @@
         <v>2015</v>
       </c>
       <c r="B71">
+        <v>70</v>
+      </c>
+      <c r="C71">
         <v>7</v>
-      </c>
-      <c r="C71">
-        <v>70</v>
       </c>
       <c r="D71" t="s">
         <v>12</v>
@@ -3616,10 +3616,10 @@
         <v>2015</v>
       </c>
       <c r="B72">
+        <v>71</v>
+      </c>
+      <c r="C72">
         <v>8</v>
-      </c>
-      <c r="C72">
-        <v>71</v>
       </c>
       <c r="D72" t="s">
         <v>12</v>
@@ -3642,10 +3642,10 @@
         <v>2015</v>
       </c>
       <c r="B73">
+        <v>72</v>
+      </c>
+      <c r="C73">
         <v>8</v>
-      </c>
-      <c r="C73">
-        <v>72</v>
       </c>
       <c r="D73" t="s">
         <v>4</v>
@@ -3668,10 +3668,10 @@
         <v>2015</v>
       </c>
       <c r="B74">
+        <v>73</v>
+      </c>
+      <c r="C74">
         <v>8</v>
-      </c>
-      <c r="C74">
-        <v>73</v>
       </c>
       <c r="D74" t="s">
         <v>10</v>
@@ -3694,10 +3694,10 @@
         <v>2015</v>
       </c>
       <c r="B75">
+        <v>74</v>
+      </c>
+      <c r="C75">
         <v>8</v>
-      </c>
-      <c r="C75">
-        <v>74</v>
       </c>
       <c r="D75" t="s">
         <v>6</v>
@@ -3720,10 +3720,10 @@
         <v>2015</v>
       </c>
       <c r="B76">
+        <v>75</v>
+      </c>
+      <c r="C76">
         <v>8</v>
-      </c>
-      <c r="C76">
-        <v>75</v>
       </c>
       <c r="D76" t="s">
         <v>5</v>
@@ -3746,10 +3746,10 @@
         <v>2015</v>
       </c>
       <c r="B77">
+        <v>76</v>
+      </c>
+      <c r="C77">
         <v>8</v>
-      </c>
-      <c r="C77">
-        <v>76</v>
       </c>
       <c r="D77" t="s">
         <v>3</v>
@@ -3772,10 +3772,10 @@
         <v>2015</v>
       </c>
       <c r="B78">
+        <v>77</v>
+      </c>
+      <c r="C78">
         <v>8</v>
-      </c>
-      <c r="C78">
-        <v>77</v>
       </c>
       <c r="D78" t="s">
         <v>9</v>
@@ -3798,10 +3798,10 @@
         <v>2015</v>
       </c>
       <c r="B79">
+        <v>78</v>
+      </c>
+      <c r="C79">
         <v>8</v>
-      </c>
-      <c r="C79">
-        <v>78</v>
       </c>
       <c r="D79" t="s">
         <v>8</v>
@@ -3824,10 +3824,10 @@
         <v>2015</v>
       </c>
       <c r="B80">
+        <v>79</v>
+      </c>
+      <c r="C80">
         <v>8</v>
-      </c>
-      <c r="C80">
-        <v>79</v>
       </c>
       <c r="D80" t="s">
         <v>7</v>
@@ -3850,10 +3850,10 @@
         <v>2015</v>
       </c>
       <c r="B81">
+        <v>80</v>
+      </c>
+      <c r="C81">
         <v>8</v>
-      </c>
-      <c r="C81">
-        <v>80</v>
       </c>
       <c r="D81" t="s">
         <v>11</v>
@@ -3876,10 +3876,10 @@
         <v>2015</v>
       </c>
       <c r="B82">
+        <v>81</v>
+      </c>
+      <c r="C82">
         <v>9</v>
-      </c>
-      <c r="C82">
-        <v>81</v>
       </c>
       <c r="D82" t="s">
         <v>11</v>
@@ -3902,10 +3902,10 @@
         <v>2015</v>
       </c>
       <c r="B83">
+        <v>82</v>
+      </c>
+      <c r="C83">
         <v>9</v>
-      </c>
-      <c r="C83">
-        <v>82</v>
       </c>
       <c r="D83" t="s">
         <v>7</v>
@@ -3928,10 +3928,10 @@
         <v>2015</v>
       </c>
       <c r="B84">
+        <v>83</v>
+      </c>
+      <c r="C84">
         <v>9</v>
-      </c>
-      <c r="C84">
-        <v>83</v>
       </c>
       <c r="D84" t="s">
         <v>8</v>
@@ -3954,10 +3954,10 @@
         <v>2015</v>
       </c>
       <c r="B85">
+        <v>84</v>
+      </c>
+      <c r="C85">
         <v>9</v>
-      </c>
-      <c r="C85">
-        <v>84</v>
       </c>
       <c r="D85" t="s">
         <v>9</v>
@@ -3980,10 +3980,10 @@
         <v>2015</v>
       </c>
       <c r="B86">
+        <v>85</v>
+      </c>
+      <c r="C86">
         <v>9</v>
-      </c>
-      <c r="C86">
-        <v>85</v>
       </c>
       <c r="D86" t="s">
         <v>3</v>
@@ -4006,10 +4006,10 @@
         <v>2015</v>
       </c>
       <c r="B87">
+        <v>86</v>
+      </c>
+      <c r="C87">
         <v>9</v>
-      </c>
-      <c r="C87">
-        <v>86</v>
       </c>
       <c r="D87" t="s">
         <v>5</v>
@@ -4032,10 +4032,10 @@
         <v>2015</v>
       </c>
       <c r="B88">
+        <v>87</v>
+      </c>
+      <c r="C88">
         <v>9</v>
-      </c>
-      <c r="C88">
-        <v>87</v>
       </c>
       <c r="D88" t="s">
         <v>6</v>
@@ -4058,10 +4058,10 @@
         <v>2015</v>
       </c>
       <c r="B89">
+        <v>88</v>
+      </c>
+      <c r="C89">
         <v>9</v>
-      </c>
-      <c r="C89">
-        <v>88</v>
       </c>
       <c r="D89" t="s">
         <v>10</v>
@@ -4084,10 +4084,10 @@
         <v>2015</v>
       </c>
       <c r="B90">
+        <v>89</v>
+      </c>
+      <c r="C90">
         <v>9</v>
-      </c>
-      <c r="C90">
-        <v>89</v>
       </c>
       <c r="D90" t="s">
         <v>4</v>
@@ -4110,10 +4110,10 @@
         <v>2015</v>
       </c>
       <c r="B91">
+        <v>90</v>
+      </c>
+      <c r="C91">
         <v>9</v>
-      </c>
-      <c r="C91">
-        <v>90</v>
       </c>
       <c r="D91" t="s">
         <v>12</v>
@@ -4136,10 +4136,10 @@
         <v>2015</v>
       </c>
       <c r="B92">
+        <v>91</v>
+      </c>
+      <c r="C92">
         <v>10</v>
-      </c>
-      <c r="C92">
-        <v>91</v>
       </c>
       <c r="D92" t="s">
         <v>12</v>
@@ -4162,10 +4162,10 @@
         <v>2015</v>
       </c>
       <c r="B93">
+        <v>92</v>
+      </c>
+      <c r="C93">
         <v>10</v>
-      </c>
-      <c r="C93">
-        <v>92</v>
       </c>
       <c r="D93" t="s">
         <v>4</v>
@@ -4188,10 +4188,10 @@
         <v>2015</v>
       </c>
       <c r="B94">
+        <v>93</v>
+      </c>
+      <c r="C94">
         <v>10</v>
-      </c>
-      <c r="C94">
-        <v>93</v>
       </c>
       <c r="D94" t="s">
         <v>10</v>
@@ -4214,10 +4214,10 @@
         <v>2015</v>
       </c>
       <c r="B95">
+        <v>94</v>
+      </c>
+      <c r="C95">
         <v>10</v>
-      </c>
-      <c r="C95">
-        <v>94</v>
       </c>
       <c r="D95" t="s">
         <v>6</v>
@@ -4240,10 +4240,10 @@
         <v>2015</v>
       </c>
       <c r="B96">
+        <v>95</v>
+      </c>
+      <c r="C96">
         <v>10</v>
-      </c>
-      <c r="C96">
-        <v>95</v>
       </c>
       <c r="D96" t="s">
         <v>5</v>
@@ -4266,10 +4266,10 @@
         <v>2015</v>
       </c>
       <c r="B97">
+        <v>96</v>
+      </c>
+      <c r="C97">
         <v>10</v>
-      </c>
-      <c r="C97">
-        <v>96</v>
       </c>
       <c r="D97" t="s">
         <v>3</v>
@@ -4292,10 +4292,10 @@
         <v>2015</v>
       </c>
       <c r="B98">
+        <v>97</v>
+      </c>
+      <c r="C98">
         <v>10</v>
-      </c>
-      <c r="C98">
-        <v>97</v>
       </c>
       <c r="D98" t="s">
         <v>9</v>
@@ -4318,10 +4318,10 @@
         <v>2015</v>
       </c>
       <c r="B99">
+        <v>98</v>
+      </c>
+      <c r="C99">
         <v>10</v>
-      </c>
-      <c r="C99">
-        <v>98</v>
       </c>
       <c r="D99" t="s">
         <v>8</v>
@@ -4344,10 +4344,10 @@
         <v>2015</v>
       </c>
       <c r="B100">
+        <v>99</v>
+      </c>
+      <c r="C100">
         <v>10</v>
-      </c>
-      <c r="C100">
-        <v>99</v>
       </c>
       <c r="D100" t="s">
         <v>7</v>
@@ -4370,10 +4370,10 @@
         <v>2015</v>
       </c>
       <c r="B101">
+        <v>100</v>
+      </c>
+      <c r="C101">
         <v>10</v>
-      </c>
-      <c r="C101">
-        <v>100</v>
       </c>
       <c r="D101" t="s">
         <v>11</v>
@@ -4396,10 +4396,10 @@
         <v>2015</v>
       </c>
       <c r="B102">
+        <v>101</v>
+      </c>
+      <c r="C102">
         <v>11</v>
-      </c>
-      <c r="C102">
-        <v>101</v>
       </c>
       <c r="D102" t="s">
         <v>11</v>
@@ -4422,10 +4422,10 @@
         <v>2015</v>
       </c>
       <c r="B103">
+        <v>102</v>
+      </c>
+      <c r="C103">
         <v>11</v>
-      </c>
-      <c r="C103">
-        <v>102</v>
       </c>
       <c r="D103" t="s">
         <v>7</v>
@@ -4448,10 +4448,10 @@
         <v>2015</v>
       </c>
       <c r="B104">
+        <v>103</v>
+      </c>
+      <c r="C104">
         <v>11</v>
-      </c>
-      <c r="C104">
-        <v>103</v>
       </c>
       <c r="D104" t="s">
         <v>8</v>
@@ -4474,10 +4474,10 @@
         <v>2015</v>
       </c>
       <c r="B105">
+        <v>104</v>
+      </c>
+      <c r="C105">
         <v>11</v>
-      </c>
-      <c r="C105">
-        <v>104</v>
       </c>
       <c r="D105" t="s">
         <v>9</v>
@@ -4500,10 +4500,10 @@
         <v>2015</v>
       </c>
       <c r="B106">
+        <v>105</v>
+      </c>
+      <c r="C106">
         <v>11</v>
-      </c>
-      <c r="C106">
-        <v>105</v>
       </c>
       <c r="D106" t="s">
         <v>3</v>
@@ -4526,10 +4526,10 @@
         <v>2015</v>
       </c>
       <c r="B107">
+        <v>106</v>
+      </c>
+      <c r="C107">
         <v>11</v>
-      </c>
-      <c r="C107">
-        <v>106</v>
       </c>
       <c r="D107" t="s">
         <v>5</v>
@@ -4552,10 +4552,10 @@
         <v>2015</v>
       </c>
       <c r="B108">
+        <v>107</v>
+      </c>
+      <c r="C108">
         <v>11</v>
-      </c>
-      <c r="C108">
-        <v>107</v>
       </c>
       <c r="D108" t="s">
         <v>6</v>
@@ -4578,10 +4578,10 @@
         <v>2015</v>
       </c>
       <c r="B109">
+        <v>108</v>
+      </c>
+      <c r="C109">
         <v>11</v>
-      </c>
-      <c r="C109">
-        <v>108</v>
       </c>
       <c r="D109" t="s">
         <v>10</v>
@@ -4604,10 +4604,10 @@
         <v>2015</v>
       </c>
       <c r="B110">
+        <v>109</v>
+      </c>
+      <c r="C110">
         <v>11</v>
-      </c>
-      <c r="C110">
-        <v>109</v>
       </c>
       <c r="D110" t="s">
         <v>4</v>
@@ -4630,10 +4630,10 @@
         <v>2015</v>
       </c>
       <c r="B111">
+        <v>110</v>
+      </c>
+      <c r="C111">
         <v>11</v>
-      </c>
-      <c r="C111">
-        <v>110</v>
       </c>
       <c r="D111" t="s">
         <v>12</v>
@@ -4656,10 +4656,10 @@
         <v>2015</v>
       </c>
       <c r="B112">
+        <v>111</v>
+      </c>
+      <c r="C112">
         <v>12</v>
-      </c>
-      <c r="C112">
-        <v>111</v>
       </c>
       <c r="D112" t="s">
         <v>12</v>
@@ -4682,10 +4682,10 @@
         <v>2015</v>
       </c>
       <c r="B113">
+        <v>112</v>
+      </c>
+      <c r="C113">
         <v>12</v>
-      </c>
-      <c r="C113">
-        <v>112</v>
       </c>
       <c r="D113" t="s">
         <v>4</v>
@@ -4708,10 +4708,10 @@
         <v>2015</v>
       </c>
       <c r="B114">
+        <v>113</v>
+      </c>
+      <c r="C114">
         <v>12</v>
-      </c>
-      <c r="C114">
-        <v>113</v>
       </c>
       <c r="D114" t="s">
         <v>10</v>
@@ -4734,10 +4734,10 @@
         <v>2015</v>
       </c>
       <c r="B115">
+        <v>114</v>
+      </c>
+      <c r="C115">
         <v>12</v>
-      </c>
-      <c r="C115">
-        <v>114</v>
       </c>
       <c r="D115" t="s">
         <v>6</v>
@@ -4760,10 +4760,10 @@
         <v>2015</v>
       </c>
       <c r="B116">
+        <v>115</v>
+      </c>
+      <c r="C116">
         <v>12</v>
-      </c>
-      <c r="C116">
-        <v>115</v>
       </c>
       <c r="D116" t="s">
         <v>5</v>
@@ -4786,10 +4786,10 @@
         <v>2015</v>
       </c>
       <c r="B117">
+        <v>116</v>
+      </c>
+      <c r="C117">
         <v>12</v>
-      </c>
-      <c r="C117">
-        <v>116</v>
       </c>
       <c r="D117" t="s">
         <v>3</v>
@@ -4812,10 +4812,10 @@
         <v>2015</v>
       </c>
       <c r="B118">
+        <v>117</v>
+      </c>
+      <c r="C118">
         <v>12</v>
-      </c>
-      <c r="C118">
-        <v>117</v>
       </c>
       <c r="D118" t="s">
         <v>9</v>
@@ -4838,10 +4838,10 @@
         <v>2015</v>
       </c>
       <c r="B119">
+        <v>118</v>
+      </c>
+      <c r="C119">
         <v>12</v>
-      </c>
-      <c r="C119">
-        <v>118</v>
       </c>
       <c r="D119" t="s">
         <v>8</v>
@@ -4864,10 +4864,10 @@
         <v>2015</v>
       </c>
       <c r="B120">
+        <v>119</v>
+      </c>
+      <c r="C120">
         <v>12</v>
-      </c>
-      <c r="C120">
-        <v>119</v>
       </c>
       <c r="D120" t="s">
         <v>7</v>
@@ -4890,10 +4890,10 @@
         <v>2015</v>
       </c>
       <c r="B121">
+        <v>120</v>
+      </c>
+      <c r="C121">
         <v>12</v>
-      </c>
-      <c r="C121">
-        <v>120</v>
       </c>
       <c r="D121" t="s">
         <v>11</v>
@@ -4916,10 +4916,10 @@
         <v>2015</v>
       </c>
       <c r="B122">
+        <v>121</v>
+      </c>
+      <c r="C122">
         <v>13</v>
-      </c>
-      <c r="C122">
-        <v>121</v>
       </c>
       <c r="D122" t="s">
         <v>11</v>
@@ -4942,10 +4942,10 @@
         <v>2015</v>
       </c>
       <c r="B123">
+        <v>122</v>
+      </c>
+      <c r="C123">
         <v>13</v>
-      </c>
-      <c r="C123">
-        <v>122</v>
       </c>
       <c r="D123" t="s">
         <v>7</v>
@@ -4968,10 +4968,10 @@
         <v>2015</v>
       </c>
       <c r="B124">
+        <v>123</v>
+      </c>
+      <c r="C124">
         <v>13</v>
-      </c>
-      <c r="C124">
-        <v>123</v>
       </c>
       <c r="D124" t="s">
         <v>8</v>
@@ -4994,10 +4994,10 @@
         <v>2015</v>
       </c>
       <c r="B125">
+        <v>124</v>
+      </c>
+      <c r="C125">
         <v>13</v>
-      </c>
-      <c r="C125">
-        <v>124</v>
       </c>
       <c r="D125" t="s">
         <v>9</v>
@@ -5020,10 +5020,10 @@
         <v>2015</v>
       </c>
       <c r="B126">
+        <v>125</v>
+      </c>
+      <c r="C126">
         <v>13</v>
-      </c>
-      <c r="C126">
-        <v>125</v>
       </c>
       <c r="D126" t="s">
         <v>3</v>
@@ -5046,10 +5046,10 @@
         <v>2015</v>
       </c>
       <c r="B127">
+        <v>126</v>
+      </c>
+      <c r="C127">
         <v>13</v>
-      </c>
-      <c r="C127">
-        <v>126</v>
       </c>
       <c r="D127" t="s">
         <v>5</v>
@@ -5072,10 +5072,10 @@
         <v>2015</v>
       </c>
       <c r="B128">
+        <v>127</v>
+      </c>
+      <c r="C128">
         <v>13</v>
-      </c>
-      <c r="C128">
-        <v>127</v>
       </c>
       <c r="D128" t="s">
         <v>6</v>
@@ -5098,10 +5098,10 @@
         <v>2015</v>
       </c>
       <c r="B129">
+        <v>128</v>
+      </c>
+      <c r="C129">
         <v>13</v>
-      </c>
-      <c r="C129">
-        <v>128</v>
       </c>
       <c r="D129" t="s">
         <v>10</v>
@@ -5124,10 +5124,10 @@
         <v>2015</v>
       </c>
       <c r="B130">
+        <v>129</v>
+      </c>
+      <c r="C130">
         <v>13</v>
-      </c>
-      <c r="C130">
-        <v>129</v>
       </c>
       <c r="D130" t="s">
         <v>4</v>
@@ -5150,10 +5150,10 @@
         <v>2015</v>
       </c>
       <c r="B131">
+        <v>130</v>
+      </c>
+      <c r="C131">
         <v>13</v>
-      </c>
-      <c r="C131">
-        <v>130</v>
       </c>
       <c r="D131" t="s">
         <v>12</v>
@@ -5176,10 +5176,10 @@
         <v>2015</v>
       </c>
       <c r="B132">
+        <v>131</v>
+      </c>
+      <c r="C132">
         <v>14</v>
-      </c>
-      <c r="C132">
-        <v>131</v>
       </c>
       <c r="D132" t="s">
         <v>12</v>
@@ -5202,10 +5202,10 @@
         <v>2015</v>
       </c>
       <c r="B133">
+        <v>132</v>
+      </c>
+      <c r="C133">
         <v>14</v>
-      </c>
-      <c r="C133">
-        <v>132</v>
       </c>
       <c r="D133" t="s">
         <v>4</v>
@@ -5228,10 +5228,10 @@
         <v>2015</v>
       </c>
       <c r="B134">
+        <v>133</v>
+      </c>
+      <c r="C134">
         <v>14</v>
-      </c>
-      <c r="C134">
-        <v>133</v>
       </c>
       <c r="D134" t="s">
         <v>10</v>
@@ -5254,10 +5254,10 @@
         <v>2015</v>
       </c>
       <c r="B135">
+        <v>134</v>
+      </c>
+      <c r="C135">
         <v>14</v>
-      </c>
-      <c r="C135">
-        <v>134</v>
       </c>
       <c r="D135" t="s">
         <v>6</v>
@@ -5280,10 +5280,10 @@
         <v>2015</v>
       </c>
       <c r="B136">
+        <v>135</v>
+      </c>
+      <c r="C136">
         <v>14</v>
-      </c>
-      <c r="C136">
-        <v>135</v>
       </c>
       <c r="D136" t="s">
         <v>5</v>
@@ -5306,10 +5306,10 @@
         <v>2015</v>
       </c>
       <c r="B137">
+        <v>136</v>
+      </c>
+      <c r="C137">
         <v>14</v>
-      </c>
-      <c r="C137">
-        <v>136</v>
       </c>
       <c r="D137" t="s">
         <v>3</v>
@@ -5332,10 +5332,10 @@
         <v>2015</v>
       </c>
       <c r="B138">
+        <v>137</v>
+      </c>
+      <c r="C138">
         <v>14</v>
-      </c>
-      <c r="C138">
-        <v>137</v>
       </c>
       <c r="D138" t="s">
         <v>9</v>
@@ -5358,10 +5358,10 @@
         <v>2015</v>
       </c>
       <c r="B139">
+        <v>138</v>
+      </c>
+      <c r="C139">
         <v>14</v>
-      </c>
-      <c r="C139">
-        <v>138</v>
       </c>
       <c r="D139" t="s">
         <v>8</v>
@@ -5384,10 +5384,10 @@
         <v>2015</v>
       </c>
       <c r="B140">
+        <v>139</v>
+      </c>
+      <c r="C140">
         <v>14</v>
-      </c>
-      <c r="C140">
-        <v>139</v>
       </c>
       <c r="D140" t="s">
         <v>7</v>
@@ -5410,10 +5410,10 @@
         <v>2015</v>
       </c>
       <c r="B141">
+        <v>140</v>
+      </c>
+      <c r="C141">
         <v>14</v>
-      </c>
-      <c r="C141">
-        <v>140</v>
       </c>
       <c r="D141" t="s">
         <v>11</v>
@@ -5436,10 +5436,10 @@
         <v>2015</v>
       </c>
       <c r="B142">
+        <v>141</v>
+      </c>
+      <c r="C142">
         <v>15</v>
-      </c>
-      <c r="C142">
-        <v>141</v>
       </c>
       <c r="D142" t="s">
         <v>11</v>
@@ -5462,10 +5462,10 @@
         <v>2015</v>
       </c>
       <c r="B143">
+        <v>142</v>
+      </c>
+      <c r="C143">
         <v>15</v>
-      </c>
-      <c r="C143">
-        <v>142</v>
       </c>
       <c r="D143" t="s">
         <v>7</v>
@@ -5488,10 +5488,10 @@
         <v>2015</v>
       </c>
       <c r="B144">
+        <v>143</v>
+      </c>
+      <c r="C144">
         <v>15</v>
-      </c>
-      <c r="C144">
-        <v>143</v>
       </c>
       <c r="D144" t="s">
         <v>8</v>
@@ -5514,10 +5514,10 @@
         <v>2015</v>
       </c>
       <c r="B145">
+        <v>144</v>
+      </c>
+      <c r="C145">
         <v>15</v>
-      </c>
-      <c r="C145">
-        <v>144</v>
       </c>
       <c r="D145" t="s">
         <v>9</v>
@@ -5540,10 +5540,10 @@
         <v>2015</v>
       </c>
       <c r="B146">
+        <v>145</v>
+      </c>
+      <c r="C146">
         <v>15</v>
-      </c>
-      <c r="C146">
-        <v>145</v>
       </c>
       <c r="D146" t="s">
         <v>3</v>
@@ -5566,10 +5566,10 @@
         <v>2015</v>
       </c>
       <c r="B147">
+        <v>146</v>
+      </c>
+      <c r="C147">
         <v>15</v>
-      </c>
-      <c r="C147">
-        <v>146</v>
       </c>
       <c r="D147" t="s">
         <v>5</v>
@@ -5592,10 +5592,10 @@
         <v>2015</v>
       </c>
       <c r="B148">
+        <v>147</v>
+      </c>
+      <c r="C148">
         <v>15</v>
-      </c>
-      <c r="C148">
-        <v>147</v>
       </c>
       <c r="D148" t="s">
         <v>6</v>
@@ -5618,10 +5618,10 @@
         <v>2015</v>
       </c>
       <c r="B149">
+        <v>148</v>
+      </c>
+      <c r="C149">
         <v>15</v>
-      </c>
-      <c r="C149">
-        <v>148</v>
       </c>
       <c r="D149" t="s">
         <v>10</v>
@@ -5644,10 +5644,10 @@
         <v>2015</v>
       </c>
       <c r="B150">
+        <v>149</v>
+      </c>
+      <c r="C150">
         <v>15</v>
-      </c>
-      <c r="C150">
-        <v>149</v>
       </c>
       <c r="D150" t="s">
         <v>4</v>
@@ -5670,10 +5670,10 @@
         <v>2015</v>
       </c>
       <c r="B151">
+        <v>150</v>
+      </c>
+      <c r="C151">
         <v>15</v>
-      </c>
-      <c r="C151">
-        <v>150</v>
       </c>
       <c r="D151" t="s">
         <v>12</v>

</xml_diff>